<commit_message>
test done, issue fixed
</commit_message>
<xml_diff>
--- a/ExcelWebAddIn_CWeb/SupportDocs/table sync logic in symbolisation.xlsx
+++ b/ExcelWebAddIn_CWeb/SupportDocs/table sync logic in symbolisation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kbrcorpau-my.sharepoint.com/personal/seamus_lu_kbr_com/Documents/Desktop/EACBOL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K149482\source\repos\ExcelWebAddIn_C\ExcelWebAddIn_CWeb\SupportDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{BFC472C9-9A88-42F3-B5A2-72F24986E7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6A9DD2B-B7D2-4FB8-8937-A57BE5E45A68}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B099F4C9-5BDC-42A1-885D-90253F3E7E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{DBCB1CE0-D54F-472B-9A12-147544FDA472}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="58">
   <si>
     <t>Change Type</t>
   </si>
@@ -44,9 +44,6 @@
     <t>handler</t>
   </si>
   <si>
-    <t>range update (single / multiple)</t>
-  </si>
-  <si>
     <t>BA</t>
   </si>
   <si>
@@ -137,31 +134,82 @@
     <t>normal</t>
   </si>
   <si>
-    <t>FILO</t>
-  </si>
-  <si>
-    <t>undo list</t>
-  </si>
-  <si>
-    <t>redo list</t>
-  </si>
-  <si>
-    <t>New change, then kill redo list, add the change to redo list accordingly</t>
-  </si>
-  <si>
-    <t>Undo, decreasing undo list, adding redo list until one mismatches</t>
-  </si>
-  <si>
-    <t>Redo, decreasinng redo list, adding undo list until one mismatches</t>
-  </si>
-  <si>
-    <t>Deafult: undo</t>
-  </si>
-  <si>
     <t>A - relocate to the previous selected range  (can be not in the rows)</t>
   </si>
   <si>
     <t>Auto select the range after change</t>
+  </si>
+  <si>
+    <t>&gt;4</t>
+  </si>
+  <si>
+    <t>AA, BA</t>
+  </si>
+  <si>
+    <t>A+A</t>
+  </si>
+  <si>
+    <t>AA, AB</t>
+  </si>
+  <si>
+    <t>A+BA, BA+A, A+A+A, A+AA,AA+A</t>
+  </si>
+  <si>
+    <t>AB+A,A+AB,A+A+A,AA+A,A+AA</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>switch case: symbol length</t>
+  </si>
+  <si>
+    <t>case 2:</t>
+  </si>
+  <si>
+    <t>if AA =&gt; compare</t>
+  </si>
+  <si>
+    <t>if BA =&gt; pass</t>
+  </si>
+  <si>
+    <t>case 3:</t>
+  </si>
+  <si>
+    <t>if ABA =&gt; compare</t>
+  </si>
+  <si>
+    <t>if else =&gt; multiple redo/undo</t>
+  </si>
+  <si>
+    <t>case 4:</t>
+  </si>
+  <si>
+    <t>case 1:</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>multiple redo/undo</t>
+  </si>
+  <si>
+    <t>range update (single / multiple continuous / multiple uncontinuous)</t>
+  </si>
+  <si>
+    <t>single undo</t>
+  </si>
+  <si>
+    <t>single redo</t>
+  </si>
+  <si>
+    <t>multiple continuous undo</t>
+  </si>
+  <si>
+    <t>multiple continuous redo</t>
   </si>
 </sst>
 </file>
@@ -260,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -277,6 +325,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,117 +349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>110359</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>159494</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9CDBC13-AE73-D9A9-2B3E-284884529C9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6960739" y="5280134"/>
-          <a:ext cx="529721" cy="404386"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>153187</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>72784</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43AFE7E0-AF00-45F5-A5F3-B4C407B39895}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4739640" y="5273827"/>
-          <a:ext cx="811924" cy="471653"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20CF7B6-C0DC-41CB-BFD4-0EDECDA6213D}">
-  <dimension ref="A1:U48"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,9 +661,11 @@
     <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
@@ -739,7 +687,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
@@ -762,50 +710,54 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="S2" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T2" s="6"/>
       <c r="U2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -830,250 +782,250 @@
       <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
+      <c r="A6" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
       <c r="U6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="T7" s="6"/>
       <c r="U7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="N8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1098,179 +1050,256 @@
       <c r="U9" s="6"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="L10" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="S10" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
+      <c r="A11" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="C18" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F19" s="18">
+        <v>2</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F20" s="18">
+        <v>3</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="D21" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1281,179 +1310,136 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="D25" s="1"/>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
       <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
       <c r="I26"/>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
       <c r="I27"/>
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D28" s="4" t="s">
-        <v>33</v>
+      <c r="D28" s="4"/>
+      <c r="G28" t="s">
+        <v>46</v>
       </c>
       <c r="I28"/>
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29"/>
+      <c r="H29" t="s">
+        <v>47</v>
+      </c>
       <c r="I29"/>
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30"/>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" t="s">
-        <v>35</v>
+      <c r="H30" t="s">
+        <v>48</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31"/>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>5</v>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="G31" t="s">
+        <v>49</v>
       </c>
       <c r="I31"/>
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>5</v>
+      <c r="D32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="H32" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
+      <c r="B36"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C39" s="3"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
+      <c r="C40" s="3"/>
+      <c r="E40" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>